<commit_message>
added advanced recipes + edited mistakes
</commit_message>
<xml_diff>
--- a/src/main/resources/Resources.xlsx
+++ b/src/main/resources/Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkbuh\java\deep-down-project\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FDE8FB3-D8AA-4C39-A2F2-1AF5806076E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63ED3123-6052-43F4-8661-181543618238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3750" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{482065D1-BD54-417D-93F5-53B3BF1318E2}"/>
+    <workbookView xWindow="7200" yWindow="3750" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{482065D1-BD54-417D-93F5-53B3BF1318E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="4" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="491">
   <si>
     <t>Title</t>
   </si>
@@ -1507,9 +1507,6 @@
   </si>
   <si>
     <t>Zeolit x 100,Compressor x 10,Steel pipe x 1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNA Fauna capsule </t>
   </si>
   <si>
     <t>DNA Fauna capsule x 3,LCD Monitor x 30,Accumulator x 1000</t>
@@ -5131,7 +5128,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>14</v>
@@ -8690,8 +8687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429C14D9-82E4-4037-A640-657D2FB3B862}">
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8862,7 +8859,7 @@
         <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8882,7 +8879,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8902,7 +8899,7 @@
         <v>108</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8922,7 +8919,7 @@
         <v>108</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8942,7 +8939,7 @@
         <v>108</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -8962,7 +8959,7 @@
         <v>108</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8982,7 +8979,7 @@
         <v>108</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9002,7 +8999,7 @@
         <v>108</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9022,7 +9019,7 @@
         <v>108</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9042,7 +9039,7 @@
         <v>108</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9062,7 +9059,7 @@
         <v>108</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9082,7 +9079,7 @@
         <v>108</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -9102,7 +9099,7 @@
         <v>108</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -9122,7 +9119,7 @@
         <v>108</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -9142,7 +9139,7 @@
         <v>108</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -9382,7 +9379,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -9482,7 +9479,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -9662,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -10062,7 +10059,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -10222,7 +10219,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -11122,7 +11119,7 @@
         <v>108</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -11182,7 +11179,7 @@
         <v>0</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -11447,7 +11444,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>387</v>

</xml_diff>